<commit_message>
Friendly names. Testing start.
</commit_message>
<xml_diff>
--- a/src/import-data/import-order-positions.xlsx
+++ b/src/import-data/import-order-positions.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jankoj\Desktop\WMS.React\src\import-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974CE39F-F5F6-4CC4-AFB9-8D98F3F4A2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E347CA-84B8-4AA4-B54D-CD5638415267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22332" yWindow="3924" windowWidth="21600" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="1404" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Kluc</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="6">
   <si>
     <t>Pozicija</t>
   </si>
@@ -36,19 +33,16 @@
     <t>Ident</t>
   </si>
   <si>
-    <t>Serijska</t>
+    <t>Količina</t>
   </si>
   <si>
-    <t>Kolicina</t>
+    <t>Št. Dokumenta</t>
   </si>
   <si>
-    <t>Beleska</t>
+    <t>Ekstra</t>
   </si>
   <si>
-    <t>Uporabnik</t>
-  </si>
-  <si>
-    <t>Vreme</t>
+    <t>CCNA</t>
   </si>
 </sst>
 </file>
@@ -84,8 +78,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,41 +362,302 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <f>2301150000001</f>
+        <v>2301150000001</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>104118</v>
+      </c>
+      <c r="D2" s="1">
+        <v>77000000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <f t="shared" ref="A3:A15" si="0">2301150000001</f>
+        <v>2301150000001</v>
+      </c>
+      <c r="B3">
+        <f>B2+1</f>
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>104134</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B15" si="1">B3+1</f>
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>104207</v>
+      </c>
+      <c r="D4" s="1">
+        <v>14000000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>104212</v>
+      </c>
+      <c r="D5" s="1">
+        <v>12000000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>104305</v>
+      </c>
+      <c r="D6" s="1">
+        <v>13000000</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="C7">
+        <v>106810</v>
+      </c>
+      <c r="D7" s="1">
+        <v>418000000</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="1"/>
         <v>7</v>
+      </c>
+      <c r="C8">
+        <v>117410</v>
+      </c>
+      <c r="D8" s="1">
+        <v>76000000</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>120006</v>
+      </c>
+      <c r="D9" s="1">
+        <v>15000000</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>251400</v>
+      </c>
+      <c r="D10" s="1">
+        <v>11000000</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>258310</v>
+      </c>
+      <c r="D11" s="1">
+        <v>11000000</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>258501</v>
+      </c>
+      <c r="D12" s="1">
+        <v>11000000</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>259908</v>
+      </c>
+      <c r="D13" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>259909</v>
+      </c>
+      <c r="D14" s="1">
+        <v>18000000</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>260001</v>
+      </c>
+      <c r="D15" s="1">
+        <v>60000000</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Asyncronous error reporting import. Versioning and unit testing.
</commit_message>
<xml_diff>
--- a/src/import-data/import-order-positions.xlsx
+++ b/src/import-data/import-order-positions.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jankoj\Desktop\WMS.React\src\import-data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717A6D02-B9BB-45CC-B6AC-B3925A518BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-23148" yWindow="1404" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -37,8 +43,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -81,32 +86,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -117,10 +117,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -158,71 +158,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -250,7 +250,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -273,11 +273,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -286,13 +286,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -302,7 +302,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -311,7 +311,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -320,7 +320,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -328,10 +328,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -396,24 +396,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -430,12 +432,13 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <f>2301150000001</f>
+        <f t="shared" ref="A2:A15" si="0">2301150000001</f>
+        <v>2301150000001</v>
       </c>
       <c r="B2" s="3">
-        <v>1</v>
+        <v>1224547468</v>
       </c>
       <c r="C2" s="3">
         <v>104118</v>
@@ -447,12 +450,14 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <f>2301150000001</f>
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
       </c>
       <c r="B3" s="3">
-        <f>B2+1</f>
+        <f t="shared" ref="B3:B15" si="1">B2+1</f>
+        <v>1224547469</v>
       </c>
       <c r="C3" s="3">
         <v>104134</v>
@@ -464,12 +469,14 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <f>2301150000001</f>
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
       </c>
       <c r="B4" s="3">
-        <f>B3+1</f>
+        <f t="shared" si="1"/>
+        <v>1224547470</v>
       </c>
       <c r="C4" s="3">
         <v>104207</v>
@@ -481,12 +488,14 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <f>2301150000001</f>
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
       </c>
       <c r="B5" s="3">
-        <f>B4+1</f>
+        <f t="shared" si="1"/>
+        <v>1224547471</v>
       </c>
       <c r="C5" s="3">
         <v>104212</v>
@@ -498,12 +507,14 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <f>2301150000001</f>
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
       </c>
       <c r="B6" s="3">
-        <f>B5+1</f>
+        <f t="shared" si="1"/>
+        <v>1224547472</v>
       </c>
       <c r="C6" s="3">
         <v>104305</v>
@@ -515,12 +526,14 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <f>2301150000001</f>
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
       </c>
       <c r="B7" s="3">
-        <f>B6+1</f>
+        <f t="shared" si="1"/>
+        <v>1224547473</v>
       </c>
       <c r="C7" s="3">
         <v>106810</v>
@@ -532,12 +545,14 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <f>2301150000001</f>
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
       </c>
       <c r="B8" s="3">
-        <f>B7+1</f>
+        <f t="shared" si="1"/>
+        <v>1224547474</v>
       </c>
       <c r="C8" s="3">
         <v>117410</v>
@@ -549,12 +564,14 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <f>2301150000001</f>
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
       </c>
       <c r="B9" s="3">
-        <f>B8+1</f>
+        <f t="shared" si="1"/>
+        <v>1224547475</v>
       </c>
       <c r="C9" s="3">
         <v>120006</v>
@@ -566,12 +583,14 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <f>2301150000001</f>
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
       </c>
       <c r="B10" s="3">
-        <f>B9+1</f>
+        <f t="shared" si="1"/>
+        <v>1224547476</v>
       </c>
       <c r="C10" s="3">
         <v>251400</v>
@@ -583,12 +602,14 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <f>2301150000001</f>
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
       </c>
       <c r="B11" s="3">
-        <f>B10+1</f>
+        <f t="shared" si="1"/>
+        <v>1224547477</v>
       </c>
       <c r="C11" s="3">
         <v>258310</v>
@@ -600,12 +621,14 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <f>2301150000001</f>
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
       </c>
       <c r="B12" s="3">
-        <f>B11+1</f>
+        <f t="shared" si="1"/>
+        <v>1224547478</v>
       </c>
       <c r="C12" s="3">
         <v>258501</v>
@@ -617,12 +640,14 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <f>2301150000001</f>
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
       </c>
       <c r="B13" s="3">
-        <f>B12+1</f>
+        <f t="shared" si="1"/>
+        <v>1224547479</v>
       </c>
       <c r="C13" s="3">
         <v>259908</v>
@@ -634,12 +659,14 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <f>2301150000001</f>
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
       </c>
       <c r="B14" s="3">
-        <f>B13+1</f>
+        <f t="shared" si="1"/>
+        <v>1224547480</v>
       </c>
       <c r="C14" s="3">
         <v>259909</v>
@@ -651,12 +678,14 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <f>2301150000001</f>
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
       </c>
       <c r="B15" s="3">
-        <f>B14+1</f>
+        <f t="shared" si="1"/>
+        <v>1224547481</v>
       </c>
       <c r="C15" s="3">
         <v>260001</v>

</xml_diff>

<commit_message>
Testing and error resolution.
</commit_message>
<xml_diff>
--- a/src/import-data/import-order-positions.xlsx
+++ b/src/import-data/import-order-positions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jankoj\Desktop\WMS.React\src\import-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A09D5C3-98A7-4C04-9965-C5B0B4BA1BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F76ADC-53F6-4289-A46F-A6E498365F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1404" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6540" yWindow="4635" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
   <si>
     <t xml:space="preserve">Številka </t>
   </si>
@@ -39,11 +39,17 @@
   <si>
     <t>CCNA</t>
   </si>
+  <si>
+    <t>Čas vpisa</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d/mm/yyyy\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -92,16 +98,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -409,22 +419,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E15"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -437,275 +448,340 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <f t="shared" ref="A2:A15" si="0">2301150000001</f>
-        <v>2301150000001</v>
-      </c>
-      <c r="B2" s="4">
-        <v>11111111111111</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="str">
+        <f>TEXT(2301150000001,"0")</f>
+        <v>2301150000001</v>
+      </c>
+      <c r="B2" s="6">
+        <f ca="1">RANDBETWEEN(1000,11111)</f>
+        <v>8736</v>
+      </c>
+      <c r="C2" s="6">
         <v>104118</v>
       </c>
       <c r="D2" s="4">
-        <v>77000000</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <f t="shared" si="0"/>
-        <v>2301150000001</v>
-      </c>
-      <c r="B3" s="4">
-        <v>11111111111</v>
-      </c>
-      <c r="C3" s="4">
+        <v>77000000.319999993</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3">
+        <f ca="1">NOW()</f>
+        <v>45324.41511898148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="str">
+        <f t="shared" ref="A3:A15" si="0">TEXT(2301150000001,"0")</f>
+        <v>2301150000001</v>
+      </c>
+      <c r="B3" s="6">
+        <f t="shared" ref="B3:B15" ca="1" si="1">RANDBETWEEN(1000,11111)</f>
+        <v>7724</v>
+      </c>
+      <c r="C3" s="6">
         <v>104134</v>
       </c>
       <c r="D3" s="4">
-        <v>10000000</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <f t="shared" si="0"/>
-        <v>2301150000001</v>
-      </c>
-      <c r="B4" s="4">
-        <f t="shared" ref="B4:B15" si="1">B3+1</f>
-        <v>11111111112</v>
-      </c>
-      <c r="C4" s="4">
+        <v>1000000.2</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F15" ca="1" si="2">NOW()</f>
+        <v>45324.41511898148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B4" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>3103</v>
+      </c>
+      <c r="C4" s="6">
         <v>104207</v>
       </c>
       <c r="D4" s="4">
         <v>14000000</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <f t="shared" si="0"/>
-        <v>2301150000001</v>
-      </c>
-      <c r="B5" s="4">
-        <f t="shared" si="1"/>
-        <v>11111111113</v>
-      </c>
-      <c r="C5" s="4">
+      <c r="E4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>45324.41511898148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B5" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>5309</v>
+      </c>
+      <c r="C5" s="6">
         <v>104212</v>
       </c>
       <c r="D5" s="4">
         <v>12000000</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <f t="shared" si="0"/>
-        <v>2301150000001</v>
-      </c>
-      <c r="B6" s="4">
-        <f t="shared" si="1"/>
-        <v>11111111114</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="E5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>45324.41511898148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B6" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>1814</v>
+      </c>
+      <c r="C6" s="6">
         <v>104305</v>
       </c>
       <c r="D6" s="4">
         <v>13000000</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <f t="shared" si="0"/>
-        <v>2301150000001</v>
-      </c>
-      <c r="B7" s="4">
-        <f t="shared" si="1"/>
-        <v>11111111115</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="E6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>45324.41511898148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B7" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>10710</v>
+      </c>
+      <c r="C7" s="6">
         <v>106810</v>
       </c>
       <c r="D7" s="4">
         <v>418000000</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <f t="shared" si="0"/>
-        <v>2301150000001</v>
-      </c>
-      <c r="B8" s="4">
-        <f t="shared" si="1"/>
-        <v>11111111116</v>
-      </c>
-      <c r="C8" s="4">
+      <c r="E7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>45324.41511898148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B8" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>4173</v>
+      </c>
+      <c r="C8" s="6">
         <v>117410</v>
       </c>
       <c r="D8" s="4">
         <v>76000000</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <f t="shared" si="0"/>
-        <v>2301150000001</v>
-      </c>
-      <c r="B9" s="4">
-        <f t="shared" si="1"/>
-        <v>11111111117</v>
-      </c>
-      <c r="C9" s="4">
+      <c r="E8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>45324.41511898148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B9" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>8762</v>
+      </c>
+      <c r="C9" s="6">
         <v>120006</v>
       </c>
       <c r="D9" s="4">
         <v>15000000</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <f t="shared" si="0"/>
-        <v>2301150000001</v>
-      </c>
-      <c r="B10" s="4">
-        <f t="shared" si="1"/>
-        <v>11111111118</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="E9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>45324.41511898148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B10" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>5811</v>
+      </c>
+      <c r="C10" s="6">
         <v>251400</v>
       </c>
       <c r="D10" s="4">
         <v>11000000</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <f t="shared" si="0"/>
-        <v>2301150000001</v>
-      </c>
-      <c r="B11" s="4">
-        <f t="shared" si="1"/>
-        <v>11111111119</v>
-      </c>
-      <c r="C11" s="4">
+      <c r="E10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>45324.41511898148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B11" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>2040</v>
+      </c>
+      <c r="C11" s="6">
         <v>258310</v>
       </c>
       <c r="D11" s="4">
         <v>11000000</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <f t="shared" si="0"/>
-        <v>2301150000001</v>
-      </c>
-      <c r="B12" s="4">
-        <f t="shared" si="1"/>
-        <v>11111111120</v>
-      </c>
-      <c r="C12" s="4">
+      <c r="E11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>45324.41511898148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B12" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>2284</v>
+      </c>
+      <c r="C12" s="6">
         <v>258501</v>
       </c>
       <c r="D12" s="4">
         <v>11000000</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <f t="shared" si="0"/>
-        <v>2301150000001</v>
-      </c>
-      <c r="B13" s="4">
-        <f t="shared" si="1"/>
-        <v>11111111121</v>
-      </c>
-      <c r="C13" s="4">
+      <c r="E12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>45324.41511898148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B13" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>10309</v>
+      </c>
+      <c r="C13" s="6">
         <v>259908</v>
       </c>
       <c r="D13" s="4">
         <v>10000000</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <f t="shared" si="0"/>
-        <v>2301150000001</v>
-      </c>
-      <c r="B14" s="4">
-        <f t="shared" si="1"/>
-        <v>11111111122</v>
-      </c>
-      <c r="C14" s="4">
+      <c r="E13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>45324.41511898148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B14" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>9016</v>
+      </c>
+      <c r="C14" s="6">
         <v>259909</v>
       </c>
       <c r="D14" s="4">
         <v>18000000</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <f t="shared" si="0"/>
-        <v>2301150000001</v>
-      </c>
-      <c r="B15" s="4">
-        <f t="shared" si="1"/>
-        <v>11111111123</v>
-      </c>
-      <c r="C15" s="4">
+      <c r="E14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>45324.41511898148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>2301150000001</v>
+      </c>
+      <c r="B15" s="6">
+        <f t="shared" ca="1" si="1"/>
+        <v>1219</v>
+      </c>
+      <c r="C15" s="6">
         <v>260001</v>
       </c>
       <c r="D15" s="4">
         <v>60000000</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="E15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>45324.41511898148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>